<commit_message>
added code pin numbers
</commit_message>
<xml_diff>
--- a/Hardware/7-23pinlist.xlsx
+++ b/Hardware/7-23pinlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WaiveCar\WaiveTelem\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{747FF8E5-B787-4573-9527-5631F94EE79D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D6CB95-4630-4F1B-B076-E96132D8B92F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5340" yWindow="2130" windowWidth="17655" windowHeight="12000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,14 +18,21 @@
     <sheet name="Differences" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'D21G18 Pinlist'!$A$1:$I$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'D21G18 Pinlist'!$A$1:$L$49</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2302" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2312" uniqueCount="683">
   <si>
     <t>Pinlist</t>
   </si>
@@ -2065,6 +2072,15 @@
   </si>
   <si>
     <t>need to strip out relevant battery charger code, GPS reset needs to be set as digital out</t>
+  </si>
+  <si>
+    <t>Program Pin Def #</t>
+  </si>
+  <si>
+    <t>Aname if any</t>
+  </si>
+  <si>
+    <t>Pins.h check</t>
   </si>
 </sst>
 </file>
@@ -12804,1243 +12820,1437 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>681</v>
+      </c>
+      <c r="B1" t="s">
+        <v>680</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>574</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>575</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>579</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>577</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>594</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>582</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>682</v>
+      </c>
+      <c r="L1" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>33</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>134</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>39</v>
-      </c>
-      <c r="E2" t="s">
-        <v>576</v>
       </c>
       <c r="G2" t="s">
         <v>576</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="I2" t="s">
+        <v>576</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>34</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
         <v>135</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
         <v>41</v>
-      </c>
-      <c r="E3" t="s">
-        <v>576</v>
       </c>
       <c r="G3" t="s">
         <v>576</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="I3" t="s">
+        <v>576</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>586</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>136</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
         <v>137</v>
-      </c>
-      <c r="E4" t="s">
-        <v>578</v>
-      </c>
-      <c r="F4" t="s">
-        <v>586</v>
       </c>
       <c r="G4" t="s">
         <v>578</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="H4" t="s">
+        <v>586</v>
+      </c>
+      <c r="I4" t="s">
+        <v>578</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>25</v>
+      </c>
+      <c r="C5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>138</v>
       </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
         <v>139</v>
-      </c>
-      <c r="E5" t="s">
-        <v>216</v>
-      </c>
-      <c r="F5" t="s">
-        <v>587</v>
       </c>
       <c r="G5" t="s">
         <v>216</v>
       </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="H5" t="s">
+        <v>587</v>
+      </c>
+      <c r="I5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>140</v>
       </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
       <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
         <v>11</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>141</v>
       </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
         <v>45</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>580</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>581</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>31</v>
+      </c>
+      <c r="C8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>142</v>
       </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
         <v>143</v>
-      </c>
-      <c r="E8" t="s">
-        <v>583</v>
       </c>
       <c r="G8" t="s">
         <v>583</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="I8" t="s">
+        <v>583</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>32</v>
+      </c>
+      <c r="C9">
         <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>144</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
       </c>
       <c r="D9" t="s">
         <v>144</v>
       </c>
       <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>144</v>
+      </c>
+      <c r="G9" t="s">
         <v>584</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>585</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>585</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>0</v>
       </c>
-      <c r="I9" t="s">
+      <c r="L9" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>588</v>
+      </c>
+      <c r="B10">
+        <v>18</v>
+      </c>
+      <c r="C10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>145</v>
       </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
         <v>146</v>
-      </c>
-      <c r="E10" t="s">
-        <v>589</v>
-      </c>
-      <c r="F10" t="s">
-        <v>588</v>
       </c>
       <c r="G10" t="s">
         <v>589</v>
       </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="H10" t="s">
+        <v>588</v>
+      </c>
+      <c r="I10" t="s">
+        <v>589</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>595</v>
+      </c>
+      <c r="B11">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
         <v>147</v>
       </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
         <v>148</v>
-      </c>
-      <c r="E11" t="s">
-        <v>596</v>
-      </c>
-      <c r="F11" t="s">
-        <v>595</v>
       </c>
       <c r="G11" t="s">
         <v>596</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="H11" t="s">
+        <v>595</v>
+      </c>
+      <c r="I11" t="s">
+        <v>596</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>598</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
         <v>149</v>
       </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
         <v>150</v>
-      </c>
-      <c r="E12" t="s">
-        <v>597</v>
-      </c>
-      <c r="F12" t="s">
-        <v>598</v>
       </c>
       <c r="G12" t="s">
         <v>597</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="H12" t="s">
+        <v>598</v>
+      </c>
+      <c r="I12" t="s">
+        <v>597</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>601</v>
+      </c>
+      <c r="B13">
+        <v>21</v>
+      </c>
+      <c r="C13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>151</v>
       </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
         <v>152</v>
-      </c>
-      <c r="E13" t="s">
-        <v>599</v>
-      </c>
-      <c r="F13" t="s">
-        <v>601</v>
       </c>
       <c r="G13" t="s">
         <v>599</v>
       </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="H13" t="s">
+        <v>601</v>
+      </c>
+      <c r="I13" t="s">
+        <v>599</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
         <v>153</v>
       </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
         <v>154</v>
-      </c>
-      <c r="E14" t="s">
-        <v>602</v>
-      </c>
-      <c r="F14" t="s">
-        <v>605</v>
       </c>
       <c r="G14" t="s">
         <v>602</v>
       </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="H14" t="s">
+        <v>605</v>
+      </c>
+      <c r="I14" t="s">
+        <v>602</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>155</v>
       </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
         <v>156</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
         <v>604</v>
       </c>
-      <c r="F15" t="s">
+      <c r="H15" t="s">
         <v>606</v>
       </c>
-      <c r="G15" t="s">
+      <c r="I15" t="s">
         <v>603</v>
       </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="J15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
         <v>157</v>
       </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
         <v>158</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>607</v>
       </c>
-      <c r="F16" t="s">
+      <c r="H16" t="s">
         <v>97</v>
       </c>
-      <c r="G16" t="s">
+      <c r="I16" t="s">
         <v>608</v>
       </c>
-      <c r="H16">
+      <c r="J16">
         <v>0</v>
       </c>
-      <c r="I16" t="s">
+      <c r="L16" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
         <v>159</v>
       </c>
-      <c r="C17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
         <v>160</v>
-      </c>
-      <c r="E17" t="s">
-        <v>609</v>
-      </c>
-      <c r="F17" t="s">
-        <v>98</v>
       </c>
       <c r="G17" t="s">
         <v>609</v>
       </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="H17" t="s">
+        <v>98</v>
+      </c>
+      <c r="I17" t="s">
+        <v>609</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
         <v>161</v>
       </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" t="s">
         <v>29</v>
-      </c>
-      <c r="E18" t="s">
-        <v>610</v>
       </c>
       <c r="G18" t="s">
         <v>610</v>
       </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="I18" t="s">
+        <v>610</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="D19" t="s">
         <v>162</v>
       </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
       <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
         <v>11</v>
       </c>
       <c r="G19" t="s">
         <v>11</v>
       </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="I19" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
         <v>163</v>
       </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
         <v>164</v>
-      </c>
-      <c r="E20" t="s">
-        <v>611</v>
-      </c>
-      <c r="F20" t="s">
-        <v>99</v>
       </c>
       <c r="G20" t="s">
         <v>611</v>
       </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="H20" t="s">
+        <v>99</v>
+      </c>
+      <c r="I20" t="s">
+        <v>611</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="D21" t="s">
         <v>165</v>
       </c>
-      <c r="C21" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
         <v>166</v>
-      </c>
-      <c r="E21" t="s">
-        <v>612</v>
-      </c>
-      <c r="F21" t="s">
-        <v>100</v>
       </c>
       <c r="G21" t="s">
         <v>612</v>
       </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="H21" t="s">
+        <v>100</v>
+      </c>
+      <c r="I21" t="s">
+        <v>612</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>26</v>
+      </c>
+      <c r="C22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
         <v>167</v>
       </c>
-      <c r="C22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
         <v>168</v>
-      </c>
-      <c r="E22" t="s">
-        <v>613</v>
       </c>
       <c r="G22" t="s">
         <v>613</v>
       </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="I22" t="s">
+        <v>613</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>27</v>
+      </c>
+      <c r="C23">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
         <v>169</v>
       </c>
-      <c r="C23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
         <v>170</v>
-      </c>
-      <c r="E23" t="s">
-        <v>614</v>
       </c>
       <c r="G23" t="s">
         <v>614</v>
       </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="I23" t="s">
+        <v>614</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>28</v>
+      </c>
+      <c r="C24">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
         <v>171</v>
       </c>
-      <c r="C24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
         <v>172</v>
       </c>
-      <c r="E24" t="s">
+      <c r="G24" t="s">
         <v>615</v>
       </c>
-      <c r="G24" t="s">
+      <c r="I24" t="s">
         <v>616</v>
       </c>
-      <c r="H24">
+      <c r="J24">
         <v>0</v>
       </c>
-      <c r="I24" t="s">
+      <c r="L24" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>29</v>
+      </c>
+      <c r="C25">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
         <v>173</v>
       </c>
-      <c r="C25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
         <v>174</v>
       </c>
-      <c r="E25" t="s">
+      <c r="G25" t="s">
         <v>618</v>
       </c>
-      <c r="G25" t="s">
+      <c r="I25" t="s">
         <v>619</v>
       </c>
-      <c r="H25">
+      <c r="J25">
         <v>0</v>
       </c>
-      <c r="I25" t="s">
+      <c r="L25" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="D26" t="s">
         <v>175</v>
       </c>
-      <c r="C26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s">
         <v>176</v>
       </c>
-      <c r="E26" t="s">
+      <c r="G26" t="s">
         <v>630</v>
       </c>
-      <c r="F26" t="s">
+      <c r="H26" t="s">
         <v>622</v>
       </c>
-      <c r="G26" t="s">
+      <c r="I26" t="s">
         <v>621</v>
       </c>
-      <c r="H26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>9</v>
+      </c>
+      <c r="C27">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="D27" t="s">
         <v>177</v>
       </c>
-      <c r="C27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
         <v>178</v>
-      </c>
-      <c r="E27" t="s">
-        <v>623</v>
-      </c>
-      <c r="F27" t="s">
-        <v>624</v>
       </c>
       <c r="G27" t="s">
         <v>623</v>
       </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="H27" t="s">
+        <v>624</v>
+      </c>
+      <c r="I27" t="s">
+        <v>623</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>24</v>
+      </c>
+      <c r="C28">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="D28" t="s">
         <v>179</v>
       </c>
-      <c r="C28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
         <v>180</v>
       </c>
-      <c r="E28" t="s">
+      <c r="G28" t="s">
         <v>625</v>
       </c>
-      <c r="G28" t="s">
+      <c r="I28" t="s">
         <v>628</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>629</v>
       </c>
-      <c r="I28" t="s">
+      <c r="K28" s="1"/>
+      <c r="L28" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="D29" t="s">
         <v>181</v>
       </c>
-      <c r="C29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s">
         <v>182</v>
-      </c>
-      <c r="E29" t="s">
-        <v>631</v>
-      </c>
-      <c r="F29" t="s">
-        <v>632</v>
       </c>
       <c r="G29" t="s">
         <v>631</v>
       </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="H29" t="s">
+        <v>632</v>
+      </c>
+      <c r="I29" t="s">
+        <v>631</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>6</v>
+      </c>
+      <c r="C30">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="D30" t="s">
         <v>183</v>
       </c>
-      <c r="C30" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s">
         <v>184</v>
-      </c>
-      <c r="E30" t="s">
-        <v>593</v>
-      </c>
-      <c r="F30" t="s">
-        <v>102</v>
       </c>
       <c r="G30" t="s">
         <v>593</v>
       </c>
-      <c r="H30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="H30" t="s">
+        <v>102</v>
+      </c>
+      <c r="I30" t="s">
+        <v>593</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>7</v>
+      </c>
+      <c r="C31">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D31" t="s">
         <v>185</v>
       </c>
-      <c r="C31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" t="s">
         <v>186</v>
-      </c>
-      <c r="E31" t="s">
-        <v>600</v>
-      </c>
-      <c r="F31" t="s">
-        <v>104</v>
       </c>
       <c r="G31" t="s">
         <v>600</v>
       </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="H31" t="s">
+        <v>104</v>
+      </c>
+      <c r="I31" t="s">
+        <v>600</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
+      <c r="D32" t="s">
         <v>187</v>
       </c>
-      <c r="C32" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" t="s">
         <v>188</v>
-      </c>
-      <c r="E32" t="s">
-        <v>591</v>
-      </c>
-      <c r="F32" t="s">
-        <v>633</v>
       </c>
       <c r="G32" t="s">
         <v>591</v>
       </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="H32" t="s">
+        <v>633</v>
+      </c>
+      <c r="I32" t="s">
+        <v>591</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="D33" t="s">
         <v>189</v>
       </c>
-      <c r="C33" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" t="s">
         <v>190</v>
-      </c>
-      <c r="E33" t="s">
-        <v>592</v>
-      </c>
-      <c r="F33" t="s">
-        <v>94</v>
       </c>
       <c r="G33" t="s">
         <v>592</v>
       </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="H33" t="s">
+        <v>94</v>
+      </c>
+      <c r="I33" t="s">
+        <v>592</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>22</v>
+      </c>
+      <c r="C34">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
+      <c r="D34" t="s">
         <v>191</v>
       </c>
-      <c r="C34" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" t="s">
         <v>117</v>
-      </c>
-      <c r="E34" t="s">
-        <v>626</v>
       </c>
       <c r="G34" t="s">
         <v>626</v>
       </c>
-      <c r="H34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="I34" t="s">
+        <v>626</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>23</v>
+      </c>
+      <c r="C35">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
+      <c r="D35" t="s">
         <v>192</v>
       </c>
-      <c r="C35" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" t="s">
         <v>116</v>
-      </c>
-      <c r="E35" t="s">
-        <v>627</v>
       </c>
       <c r="G35" t="s">
         <v>627</v>
       </c>
-      <c r="H35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="I35" t="s">
+        <v>627</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C36">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
+      <c r="D36" t="s">
         <v>193</v>
       </c>
-      <c r="C36" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" t="s">
-        <v>11</v>
-      </c>
       <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" t="s">
         <v>11</v>
       </c>
       <c r="G36" t="s">
         <v>11</v>
       </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="I36" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C37">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
+      <c r="D37" t="s">
         <v>194</v>
       </c>
-      <c r="C37" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" t="s">
         <v>29</v>
       </c>
-      <c r="E37" t="s">
+      <c r="G37" t="s">
         <v>634</v>
       </c>
-      <c r="G37" t="s">
+      <c r="I37" t="s">
         <v>610</v>
       </c>
-      <c r="H37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="J37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>14</v>
+      </c>
+      <c r="C38">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
+      <c r="D38" t="s">
         <v>195</v>
       </c>
-      <c r="C38" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" t="s">
         <v>129</v>
-      </c>
-      <c r="E38" t="s">
-        <v>635</v>
-      </c>
-      <c r="F38" t="s">
-        <v>637</v>
       </c>
       <c r="G38" t="s">
         <v>635</v>
       </c>
-      <c r="H38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="H38" t="s">
+        <v>637</v>
+      </c>
+      <c r="I38" t="s">
+        <v>635</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>13</v>
+      </c>
+      <c r="C39">
         <v>38</v>
       </c>
-      <c r="B39" t="s">
+      <c r="D39" t="s">
         <v>196</v>
       </c>
-      <c r="C39" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" t="s">
         <v>132</v>
-      </c>
-      <c r="E39" t="s">
-        <v>636</v>
-      </c>
-      <c r="F39" t="s">
-        <v>638</v>
       </c>
       <c r="G39" t="s">
         <v>636</v>
       </c>
-      <c r="H39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="H39" t="s">
+        <v>638</v>
+      </c>
+      <c r="I39" t="s">
+        <v>636</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>30</v>
+      </c>
+      <c r="C40">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
+      <c r="D40" t="s">
         <v>197</v>
       </c>
-      <c r="C40" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" t="s">
         <v>198</v>
       </c>
-      <c r="E40" t="s">
+      <c r="G40" t="s">
         <v>639</v>
       </c>
-      <c r="G40" t="s">
+      <c r="I40" t="s">
         <v>640</v>
       </c>
-      <c r="H40">
+      <c r="J40">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C41">
         <v>40</v>
       </c>
-      <c r="B41" t="s">
+      <c r="D41" t="s">
         <v>199</v>
       </c>
-      <c r="C41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" t="s">
         <v>90</v>
-      </c>
-      <c r="E41" t="s">
-        <v>641</v>
       </c>
       <c r="G41" t="s">
         <v>641</v>
       </c>
-      <c r="H41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="I41" t="s">
+        <v>641</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>35</v>
+      </c>
+      <c r="C42">
         <v>41</v>
       </c>
-      <c r="B42" t="s">
+      <c r="D42" t="s">
         <v>200</v>
       </c>
-      <c r="C42" t="s">
-        <v>10</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" t="s">
         <v>201</v>
-      </c>
-      <c r="E42" t="s">
-        <v>642</v>
       </c>
       <c r="G42" t="s">
         <v>642</v>
       </c>
-      <c r="H42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="I42" t="s">
+        <v>642</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C43">
         <v>42</v>
       </c>
-      <c r="B43" t="s">
+      <c r="D43" t="s">
         <v>202</v>
       </c>
-      <c r="C43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" t="s">
-        <v>11</v>
-      </c>
       <c r="E43" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" t="s">
         <v>11</v>
       </c>
       <c r="G43" t="s">
         <v>11</v>
       </c>
-      <c r="H43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="I43" t="s">
+        <v>11</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C44">
         <v>43</v>
       </c>
-      <c r="B44" t="s">
+      <c r="D44" t="s">
         <v>203</v>
       </c>
-      <c r="C44" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" t="s">
         <v>56</v>
-      </c>
-      <c r="E44" t="s">
-        <v>634</v>
       </c>
       <c r="G44" t="s">
         <v>634</v>
       </c>
-      <c r="H44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="I44" t="s">
+        <v>634</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C45">
         <v>44</v>
       </c>
-      <c r="B45" t="s">
+      <c r="D45" t="s">
         <v>204</v>
       </c>
-      <c r="C45" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" t="s">
         <v>29</v>
-      </c>
-      <c r="E45" t="s">
-        <v>634</v>
       </c>
       <c r="G45" t="s">
         <v>634</v>
       </c>
-      <c r="H45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="I45" t="s">
+        <v>634</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C46">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
+      <c r="D46" t="s">
         <v>205</v>
       </c>
-      <c r="C46" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" t="s">
         <v>206</v>
-      </c>
-      <c r="E46" t="s">
-        <v>643</v>
       </c>
       <c r="G46" t="s">
         <v>643</v>
       </c>
-      <c r="H46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="I46" t="s">
+        <v>643</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C47">
         <v>46</v>
       </c>
-      <c r="B47" t="s">
+      <c r="D47" t="s">
         <v>207</v>
       </c>
-      <c r="C47" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" t="s">
         <v>208</v>
-      </c>
-      <c r="E47" t="s">
-        <v>643</v>
       </c>
       <c r="G47" t="s">
         <v>643</v>
       </c>
-      <c r="H47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="I47" t="s">
+        <v>643</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>570</v>
+      </c>
+      <c r="B48">
+        <v>16</v>
+      </c>
+      <c r="C48">
         <v>47</v>
       </c>
-      <c r="B48" t="s">
+      <c r="D48" t="s">
         <v>209</v>
       </c>
-      <c r="C48" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" t="s">
         <v>210</v>
-      </c>
-      <c r="E48" t="s">
-        <v>644</v>
-      </c>
-      <c r="F48" t="s">
-        <v>570</v>
       </c>
       <c r="G48" t="s">
         <v>644</v>
       </c>
-      <c r="H48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="H48" t="s">
+        <v>570</v>
+      </c>
+      <c r="I48" t="s">
+        <v>644</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>571</v>
+      </c>
+      <c r="B49">
+        <v>17</v>
+      </c>
+      <c r="C49">
         <v>48</v>
       </c>
-      <c r="B49" t="s">
+      <c r="D49" t="s">
         <v>211</v>
       </c>
-      <c r="C49" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" t="s">
         <v>212</v>
-      </c>
-      <c r="E49" t="s">
-        <v>590</v>
-      </c>
-      <c r="F49" t="s">
-        <v>571</v>
       </c>
       <c r="G49" t="s">
         <v>590</v>
       </c>
-      <c r="H49">
+      <c r="H49" t="s">
+        <v>571</v>
+      </c>
+      <c r="I49" t="s">
+        <v>590</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="K49">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L49" xr:uid="{1643801E-FF1E-4B60-9685-3E91C835F634}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -14050,12 +14260,12 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>

</xml_diff>